<commit_message>
Done Cải tiến CLS
</commit_message>
<xml_diff>
--- a/DataTest/Khám bệnh - CDDV/TC_02.xlsx
+++ b/DataTest/Khám bệnh - CDDV/TC_02.xlsx
@@ -1,318 +1,284 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\HIS api automation\DataTest\Khám bệnh - CDDV\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\HIS api automation\DataTest\Khám bệnh - CDDV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FD041D0-B7BB-4DD9-89A8-02641564C65C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE116F0-656C-49EA-B761-3D59A972A92F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{794CA7EE-973C-4E52-B2EA-D86EA806D076}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Check" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="106">
-  <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>LastName</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="100">
+  <si>
+    <t>DxSymptom</t>
+  </si>
+  <si>
+    <t>InitialDxICD</t>
+  </si>
+  <si>
+    <t>InitialDxText</t>
+  </si>
+  <si>
+    <t>DxICD</t>
+  </si>
+  <si>
+    <t>DxText</t>
+  </si>
+  <si>
+    <t>DxByStaffId</t>
+  </si>
+  <si>
+    <t>CreateById</t>
+  </si>
+  <si>
+    <t>TxInstruction</t>
+  </si>
+  <si>
+    <t>MedRcdNo</t>
+  </si>
+  <si>
+    <t>IcdCode</t>
+  </si>
+  <si>
+    <t>ICDReason</t>
+  </si>
+  <si>
+    <t>TxVisitId</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Attribute1</t>
+  </si>
+  <si>
+    <t>VisitEntryId</t>
+  </si>
+  <si>
+    <t>CreateByStaffName</t>
+  </si>
+  <si>
+    <t>PxItems</t>
+  </si>
+  <si>
+    <t>ServiceId</t>
+  </si>
+  <si>
+    <t>Code</t>
+  </si>
+  <si>
+    <t>TypeL1</t>
+  </si>
+  <si>
+    <t>TypeL2</t>
+  </si>
+  <si>
+    <t>TypeL3</t>
+  </si>
+  <si>
+    <t>TypeL4</t>
+  </si>
+  <si>
+    <t>Category</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>Unit</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>InsServiceName</t>
+  </si>
+  <si>
+    <t>Attribute2</t>
+  </si>
+  <si>
+    <t>NationalCode</t>
   </si>
   <si>
     <t>Status</t>
   </si>
   <si>
+    <t>InsPrice</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>PriceId</t>
+  </si>
+  <si>
+    <t>ServiceGroupName</t>
+  </si>
+  <si>
+    <t>LabExams</t>
+  </si>
+  <si>
+    <t>CreatedBy</t>
+  </si>
+  <si>
+    <t>ContentHash</t>
+  </si>
+  <si>
+    <t>IsPassOnWarning</t>
+  </si>
+  <si>
+    <t>RefNo</t>
+  </si>
+  <si>
+    <t>LabReqNotes</t>
+  </si>
+  <si>
+    <t>Attribute</t>
+  </si>
+  <si>
+    <t>Status.1</t>
+  </si>
+  <si>
+    <t>LabExId</t>
+  </si>
+  <si>
+    <t>MedServiceId</t>
+  </si>
+  <si>
+    <t>PriceId.1</t>
+  </si>
+  <si>
+    <t>Qty</t>
+  </si>
+  <si>
+    <t>Price.1</t>
+  </si>
+  <si>
+    <t>InsPrice.1</t>
+  </si>
+  <si>
+    <t>InsPriceRatio</t>
+  </si>
+  <si>
+    <t>ByProviderId</t>
+  </si>
+  <si>
+    <t>DiscAmtSeq</t>
+  </si>
+  <si>
+    <t>MedServiceTypeL0</t>
+  </si>
+  <si>
+    <t>MedServiceTypeL2</t>
+  </si>
+  <si>
+    <t>MedServiceTypeL3</t>
+  </si>
+  <si>
+    <t>NonSubclinical</t>
+  </si>
+  <si>
+    <t>TypeL0Code</t>
+  </si>
+  <si>
+    <t>ByProviderCode</t>
+  </si>
+  <si>
+    <t>ByProviderName</t>
+  </si>
+  <si>
+    <t>ServiceGroupName.1</t>
+  </si>
+  <si>
+    <t>ServiceTypeL3Name</t>
+  </si>
+  <si>
+    <t>ServiceCode</t>
+  </si>
+  <si>
+    <t>ServiceName</t>
+  </si>
+  <si>
+    <t>InsBenefitTypeName</t>
+  </si>
+  <si>
+    <t>ReqDate</t>
+  </si>
+  <si>
+    <t>AttrString</t>
+  </si>
+  <si>
+    <t>PaidAttrString</t>
+  </si>
+  <si>
+    <t>ServiceTypeOrderIndex</t>
+  </si>
+  <si>
+    <t>MedItemType</t>
+  </si>
+  <si>
+    <t>MedItem</t>
+  </si>
+  <si>
+    <t>Checked</t>
+  </si>
+  <si>
+    <t>TotalInvoiceAmtRound</t>
+  </si>
+  <si>
+    <t>TotalReceiptAmtRound</t>
+  </si>
+  <si>
+    <t>PtAmt</t>
+  </si>
+  <si>
+    <t>PtAmtRound</t>
+  </si>
+  <si>
+    <t>PtAmtPaid</t>
+  </si>
+  <si>
+    <t>PtCoPayAmt</t>
+  </si>
+  <si>
+    <t>PtCoPayAmtRound</t>
+  </si>
+  <si>
+    <t>InsAmt</t>
+  </si>
+  <si>
+    <t>InsAmtRound</t>
+  </si>
+  <si>
+    <t>DiscAmt</t>
+  </si>
+  <si>
+    <t>ReqBy</t>
+  </si>
+  <si>
     <t>FullAddress</t>
   </si>
   <si>
-    <t>InsCardNo</t>
-  </si>
-  <si>
-    <t>Attribute</t>
-  </si>
-  <si>
-    <t>InsBenefitType</t>
-  </si>
-  <si>
-    <t>InsBenefitRatio</t>
-  </si>
-  <si>
-    <t>CreateById</t>
-  </si>
-  <si>
-    <t>MedServiceId</t>
-  </si>
-  <si>
-    <t>PriceId</t>
-  </si>
-  <si>
-    <t>LabExams</t>
-  </si>
-  <si>
-    <t>CreatedBy</t>
-  </si>
-  <si>
-    <t>ContentHash</t>
-  </si>
-  <si>
-    <t>InsBenefitTypeName</t>
-  </si>
-  <si>
-    <t>CreateByStaffName</t>
+    <t>Bệnh tả, không đặc hiệu</t>
+  </si>
+  <si>
+    <t>A00.9</t>
   </si>
   <si>
     <t>Quách Bảo Hưng</t>
-  </si>
-  <si>
-    <t>DN4127460129104</t>
-  </si>
-  <si>
-    <t>DxSymptom</t>
-  </si>
-  <si>
-    <t>InitialDxICD</t>
-  </si>
-  <si>
-    <t>InitialDxText</t>
-  </si>
-  <si>
-    <t>DxICD</t>
-  </si>
-  <si>
-    <t>DxText</t>
-  </si>
-  <si>
-    <t>DxByStaffId</t>
-  </si>
-  <si>
-    <t>TxInstruction</t>
-  </si>
-  <si>
-    <t>MedRcdNo</t>
-  </si>
-  <si>
-    <t>IcdCode</t>
-  </si>
-  <si>
-    <t>ICDReason</t>
-  </si>
-  <si>
-    <t>TxVisitId</t>
-  </si>
-  <si>
-    <t>Type</t>
-  </si>
-  <si>
-    <t>Attribute1</t>
-  </si>
-  <si>
-    <t>VisitEntryId</t>
-  </si>
-  <si>
-    <t>PxItems</t>
-  </si>
-  <si>
-    <t>ServiceId</t>
-  </si>
-  <si>
-    <t>Code</t>
-  </si>
-  <si>
-    <t>TypeL1</t>
-  </si>
-  <si>
-    <t>TypeL2</t>
-  </si>
-  <si>
-    <t>TypeL3</t>
-  </si>
-  <si>
-    <t>TypeL4</t>
-  </si>
-  <si>
-    <t>Category</t>
-  </si>
-  <si>
-    <t>Rank</t>
-  </si>
-  <si>
-    <t>Unit</t>
-  </si>
-  <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>InsServiceName</t>
-  </si>
-  <si>
-    <t>Attribute2</t>
-  </si>
-  <si>
-    <t>NationalCode</t>
-  </si>
-  <si>
-    <t>InsPrice</t>
-  </si>
-  <si>
-    <t>Price</t>
-  </si>
-  <si>
-    <t>ServiceGroupName</t>
-  </si>
-  <si>
-    <t>IsPassOnWarning</t>
-  </si>
-  <si>
-    <t>RefNo</t>
-  </si>
-  <si>
-    <t>LabReqNotes</t>
-  </si>
-  <si>
-    <t>Status.1</t>
-  </si>
-  <si>
-    <t>LabExId</t>
-  </si>
-  <si>
-    <t>PriceId.1</t>
-  </si>
-  <si>
-    <t>Qty</t>
-  </si>
-  <si>
-    <t>Price.1</t>
-  </si>
-  <si>
-    <t>InsPrice.1</t>
-  </si>
-  <si>
-    <t>InsPriceRatio</t>
-  </si>
-  <si>
-    <t>ByProviderId</t>
-  </si>
-  <si>
-    <t>DiscAmtSeq</t>
-  </si>
-  <si>
-    <t>MedServiceTypeL0</t>
-  </si>
-  <si>
-    <t>MedServiceTypeL2</t>
-  </si>
-  <si>
-    <t>MedServiceTypeL3</t>
-  </si>
-  <si>
-    <t>NonSubclinical</t>
-  </si>
-  <si>
-    <t>TypeL0Code</t>
-  </si>
-  <si>
-    <t>ByProviderCode</t>
-  </si>
-  <si>
-    <t>ByProviderName</t>
-  </si>
-  <si>
-    <t>ServiceGroupName.1</t>
-  </si>
-  <si>
-    <t>ServiceTypeL3Name</t>
-  </si>
-  <si>
-    <t>ServiceCode</t>
-  </si>
-  <si>
-    <t>ServiceName</t>
-  </si>
-  <si>
-    <t>ReqDate</t>
-  </si>
-  <si>
-    <t>AttrString</t>
-  </si>
-  <si>
-    <t>PaidAttrString</t>
-  </si>
-  <si>
-    <t>ServiceTypeOrderIndex</t>
-  </si>
-  <si>
-    <t>MedItemType</t>
-  </si>
-  <si>
-    <t>MedItem</t>
-  </si>
-  <si>
-    <t>Checked</t>
-  </si>
-  <si>
-    <t>TotalInvoiceAmtRound</t>
-  </si>
-  <si>
-    <t>TotalReceiptAmtRound</t>
-  </si>
-  <si>
-    <t>PtAmt</t>
-  </si>
-  <si>
-    <t>PtAmtRound</t>
-  </si>
-  <si>
-    <t>PtAmtPaid</t>
-  </si>
-  <si>
-    <t>PtCoPayAmt</t>
-  </si>
-  <si>
-    <t>PtCoPayAmtRound</t>
-  </si>
-  <si>
-    <t>InsAmt</t>
-  </si>
-  <si>
-    <t>InsAmtRound</t>
-  </si>
-  <si>
-    <t>DiscAmt</t>
-  </si>
-  <si>
-    <t>ReqBy</t>
-  </si>
-  <si>
-    <t>Bệnh tả, không đặc hiệu</t>
-  </si>
-  <si>
-    <t>A00.9</t>
   </si>
   <si>
     <t>knt1</t>
@@ -361,7 +327,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -375,6 +341,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -384,7 +355,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -407,13 +378,31 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -729,296 +718,297 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E64A327E-43DD-469F-A788-E92153460493}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:CE2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L7" sqref="L7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection sqref="A1:XFD2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10" customWidth="1"/>
-    <col min="8" max="8" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="16" max="17" width="35.77734375" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="52.77734375" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="13.21875" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="32.109375" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="61.21875" bestFit="1" customWidth="1"/>
-    <col min="55" max="55" width="14.33203125" bestFit="1" customWidth="1"/>
-    <col min="59" max="59" width="231.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="35.7109375" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="52.7109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="32.140625" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="61.28515625" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="14.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="60" max="60" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:83" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:83" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>20</v>
+        <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>21</v>
+        <v>3</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>25</v>
-      </c>
       <c r="J1" s="1" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>28</v>
+        <v>11</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>30</v>
+        <v>13</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>31</v>
+        <v>14</v>
       </c>
       <c r="P1" s="1" t="s">
         <v>15</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="AH1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="AI1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="AJ1" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="AK1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="AL1" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="AM1" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="AN1" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="AO1" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="Z1" s="1" t="s">
+      <c r="AP1" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="AA1" s="1" t="s">
+      <c r="AQ1" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="AB1" s="1" t="s">
+      <c r="AR1" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="AC1" s="1" t="s">
+      <c r="AS1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="AD1" s="1" t="s">
+      <c r="AT1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="AE1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="AF1" s="1" t="s">
+      <c r="AU1" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="AG1" s="1" t="s">
+      <c r="AV1" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="AH1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="AI1" s="1" t="s">
+      <c r="AW1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="AJ1" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="AK1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="AL1" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="AM1" s="1" t="s">
+      <c r="AX1" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AN1" s="1" t="s">
+      <c r="AY1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="AO1" s="1" t="s">
+      <c r="AZ1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="AP1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="AQ1" s="1" t="s">
+      <c r="BA1" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="AR1" s="1" t="s">
+      <c r="BB1" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="AS1" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="AT1" s="1" t="s">
+      <c r="BC1" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="AU1" s="1" t="s">
+      <c r="BD1" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="AV1" s="1" t="s">
+      <c r="BE1" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="AW1" s="1" t="s">
+      <c r="BF1" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="AX1" s="1" t="s">
+      <c r="BG1" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="AY1" s="1" t="s">
+      <c r="BH1" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="AZ1" s="1" t="s">
+      <c r="BI1" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="BA1" s="1" t="s">
+      <c r="BJ1" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="BB1" s="1" t="s">
+      <c r="BK1" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="BC1" s="1" t="s">
+      <c r="BL1" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="BD1" s="1" t="s">
+      <c r="BM1" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="BE1" s="1" t="s">
+      <c r="BN1" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="BF1" s="1" t="s">
+      <c r="BO1" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="BG1" s="1" t="s">
+      <c r="BP1" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="BH1" s="1" t="s">
+      <c r="BQ1" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="BI1" s="1" t="s">
+      <c r="BR1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="BJ1" s="1" t="s">
+      <c r="BS1" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="BK1" s="1" t="s">
+      <c r="BT1" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="BL1" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="BM1" s="1" t="s">
+      <c r="BU1" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="BN1" s="1" t="s">
+      <c r="BV1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="BO1" s="1" t="s">
+      <c r="BW1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="BP1" s="1" t="s">
+      <c r="BX1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="BQ1" s="1" t="s">
+      <c r="BY1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="BR1" s="1" t="s">
+      <c r="BZ1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="BS1" s="1" t="s">
+      <c r="CA1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="BT1" s="1" t="s">
+      <c r="CB1" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="BU1" s="1" t="s">
+      <c r="CC1" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="BV1" s="1" t="s">
+      <c r="CD1" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="BW1" s="1" t="s">
+      <c r="CE1" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="BX1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:83" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>83</v>
       </c>
-      <c r="BY1" s="1" t="s">
+      <c r="B2" t="s">
         <v>84</v>
       </c>
-      <c r="BZ1" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="CA1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="CB1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="CC1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="CD1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="CE1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:83" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>90</v>
-      </c>
-      <c r="B2" t="s">
-        <v>91</v>
-      </c>
       <c r="C2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="E2" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="F2">
         <v>3839</v>
@@ -1039,13 +1029,13 @@
         <v>17437</v>
       </c>
       <c r="P2" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="R2">
         <v>4803</v>
       </c>
       <c r="S2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="T2">
         <v>13</v>
@@ -1066,13 +1056,13 @@
         <v>1</v>
       </c>
       <c r="Z2" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="AA2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AB2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AC2">
         <v>1024</v>
@@ -1093,13 +1083,13 @@
         <v>1094172</v>
       </c>
       <c r="AL2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="AM2" t="b">
         <v>0</v>
       </c>
       <c r="AN2" t="s">
-        <v>97</v>
+        <v>91</v>
       </c>
       <c r="AP2">
         <v>1</v>
@@ -1135,31 +1125,31 @@
         <v>0</v>
       </c>
       <c r="BF2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BL2" t="s">
         <v>98</v>
       </c>
-      <c r="BG2" t="s">
+      <c r="BN2" t="s">
         <v>99</v>
       </c>
-      <c r="BH2" t="s">
-        <v>100</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>101</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>103</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>104</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>105</v>
-      </c>
       <c r="BO2" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="BP2">
         <v>0</v>
@@ -1198,56 +1188,51 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FBC7F63F-8A09-4317-BC6C-1379C0A58D70}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:F2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2">
+        <v>1095239</v>
+      </c>
+      <c r="C2">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1913</v>
-      </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
       <c r="D2">
-        <v>3839</v>
-      </c>
-      <c r="E2">
-        <v>80</v>
-      </c>
-      <c r="F2">
-        <v>2</v>
+        <v>624000</v>
+      </c>
+      <c r="E2" t="s">
+        <v>96</v>
+      </c>
+      <c r="F2" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>